<commit_message>
update readme and graphs in excel
</commit_message>
<xml_diff>
--- a/out/stir_daily_system_wide_with GRAPHS_22Oct25.xlsx
+++ b/out/stir_daily_system_wide_with GRAPHS_22Oct25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7d62234183fd3ba/Documents/GitHub/kerbel-long-term-impacts/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3109FC4A-BD15-44FB-B1BB-C01FAB71276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F2DA776-91FC-45BF-B4BE-1085562B1E8E}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{3109FC4A-BD15-44FB-B1BB-C01FAB71276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83CB4F38-4E55-4379-BB2E-9966B92C634D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="780" windowWidth="29040" windowHeight="15720" xr2:uid="{95A4D3B7-9F89-4514-B226-E93CDF5B25B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{95A4D3B7-9F89-4514-B226-E93CDF5B25B1}"/>
   </bookViews>
   <sheets>
     <sheet name="stir_daily_system_wide" sheetId="1" r:id="rId1"/>
@@ -659,8 +659,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -677,28 +677,43 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:noFill/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>stir_daily_system_wide!$A$2:$A$174</c:f>
               <c:numCache>
@@ -1225,8 +1240,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>stir_daily_system_wide!$U$2:$U$174</c:f>
               <c:numCache>
@@ -1753,8 +1768,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-24DF-40AF-B0D9-309C2EB0DBC7}"/>
@@ -1776,28 +1790,43 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>stir_daily_system_wide!$A$2:$A$174</c:f>
               <c:numCache>
@@ -2324,8 +2353,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>stir_daily_system_wide!$W$2:$W$174</c:f>
               <c:numCache>
@@ -2852,8 +2881,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-24DF-40AF-B0D9-309C2EB0DBC7}"/>
@@ -2875,28 +2903,43 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>stir_daily_system_wide!$A$2:$A$174</c:f>
               <c:numCache>
@@ -3423,8 +3466,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>stir_daily_system_wide!$Y$2:$Y$174</c:f>
               <c:numCache>
@@ -3951,8 +3994,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-24DF-40AF-B0D9-309C2EB0DBC7}"/>
@@ -3969,8 +4011,8 @@
         </c:dLbls>
         <c:axId val="1258194463"/>
         <c:axId val="1258196383"/>
-      </c:scatterChart>
-      <c:valAx>
+      </c:areaChart>
+      <c:dateAx>
         <c:axId val="1258194463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -3997,14 +4039,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4016,8 +4052,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4030,14 +4066,16 @@
         </c:txPr>
         <c:crossAx val="1258196383"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="1258196383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -4060,11 +4098,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -4092,11 +4130,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -4112,6 +4150,33 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1258194463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -4125,7 +4190,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4142,8 +4207,8 @@
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -7594,7 +7659,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -7666,9 +7731,42 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1258194463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -7837,18 +7935,18 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="280">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -7856,16 +7954,16 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7878,7 +7976,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -7894,7 +7992,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -7902,8 +8000,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -7937,36 +8035,62 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="15875" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -7978,27 +8102,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="2"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
@@ -8018,20 +8145,18 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8041,7 +8166,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -8050,14 +8175,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8066,17 +8190,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -8085,17 +8209,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -8104,21 +8227,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -8137,17 +8254,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -8156,17 +8272,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -8175,17 +8291,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -8195,8 +8310,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8206,7 +8321,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -8214,7 +8329,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -8223,10 +8338,21 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -8234,17 +8360,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -8254,27 +8380,26 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="2"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -8284,8 +8409,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8295,20 +8420,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8318,21 +8442,10 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8340,14 +8453,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9268,8 +9375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2A62A6-3D73-4CE5-ABB5-A10C35402FCA}">
   <dimension ref="A1:Z174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection sqref="A1:Z1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AG42" sqref="AG42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
merge stir and wq kinda working
</commit_message>
<xml_diff>
--- a/out/stir_daily_system_wide_with GRAPHS_22Oct25.xlsx
+++ b/out/stir_daily_system_wide_with GRAPHS_22Oct25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7d62234183fd3ba/Documents/GitHub/kerbel-long-term-impacts/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{3109FC4A-BD15-44FB-B1BB-C01FAB71276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13FD767F-E0BB-4248-ADEF-37CB55D7C87C}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{3109FC4A-BD15-44FB-B1BB-C01FAB71276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EDFD4D9-34B1-44C7-A3E4-6655D2C4A1AD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{95A4D3B7-9F89-4514-B226-E93CDF5B25B1}"/>
   </bookViews>
@@ -11512,6 +11512,1940 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stir_daily_system_wide!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CT_STIR_Sum_Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>stir_daily_system_wide!$U$2:$U$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="173"/>
+                <c:pt idx="0">
+                  <c:v>123.43499999999899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154.63499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175.435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>177.62875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179.82249999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>186.32249999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>186.32249999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>186.32249999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189.57249999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>204.19749999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>210.69749999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>241.41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>280.409999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>102.37499999999901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>133.57499999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>154.375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>154.375</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>177.36874999999901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>177.36874999999901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>183.86874999999901</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>185.33124999999899</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>186.79374999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>186.79374999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>186.79374999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>204.66874999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>211.16874999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>241.88124999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>344.256249999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33.393749999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36.643749999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39.893749999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>39.893749999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>54.518749999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>54.518749999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>61.018749999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66.478749999999906</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>168.85374999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>171.04749999999899</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.1937499999999899</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.59375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>33.653750000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>58.841250000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>62.091250000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>62.091250000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>76.716250000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>113.92874999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>141.375</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>143.56874999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>143.56874999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>169.8125</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>173.0625</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>173.0625</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>187.6875</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>194.1875</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>224.9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>353.79499999999899</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.1937499999999899</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>12.59375</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>15.84375</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>41.03125</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>47.368749999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>47.368749999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>53.868749999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>69.224999999999994</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>69.224999999999994</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>69.224999999999994</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>104.568749999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>117.162499999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>120.412499999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>143.40624999999901</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>143.40624999999901</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>146.65624999999901</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>161.28124999999901</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>167.78124999999901</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>173.24124999999901</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>102.37499999999901</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>104.568749999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>117.162499999999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>119.35624999999899</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>122.60624999999899</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>137.23124999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>138.69374999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>141.94374999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>156.56874999999999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>158.76249999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>173.38749999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>179.88749999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>186.38749999999999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>197.30749999999901</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>197.30749999999901</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>225.74499999999901</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>232.08249999999899</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>27.31625</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>48.376249999999999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>150.751249999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>152.94499999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>163.344999999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>26.243749999999999</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>31.6875</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>38.1875</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>68.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>74.36</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>107.834999999999</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>120.428749999999</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>122.62249999999899</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>124.816249999999</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>128.066249999999</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>163.49124999999901</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>165.68499999999901</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>167.878749999999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>171.128749999999</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>171.128749999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>174.378749999999</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>203.628749999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>203.628749999999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>210.128749999999</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>240.84124999999901</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>246.30124999999899</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>251.76124999999999</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>272.821249999999</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>377.39</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>389.98374999999999</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>38.674999999999997</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>40.868749999999999</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>44.118749999999999</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>44.118749999999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>76.618750000000006</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>83.118750000000006</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>98.474999999999994</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>206.30999999999901</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>208.503749999999</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.1937499999999899</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>12.59375</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>38.837499999999999</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>41.03125</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>47.53125</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>47.53125</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>50.78125</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>67.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>74.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>82.81</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>112.14125</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>21.06</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>123.43499999999899</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>125.628749999999</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>127.822499999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>138.2225</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2.1937499999999899</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>6.5812499999999901</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>9.8312499999999901</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>9.8312499999999901</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>32.824999999999903</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>36.074999999999903</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>39.324999999999903</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>70.037499999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C15E-4A2C-8307-4062D2034C2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stir_daily_system_wide!$W$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ST_STIR_Sum_Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>stir_daily_system_wide!$W$2:$W$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="173"/>
+                <c:pt idx="0">
+                  <c:v>4.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66.462500000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66.462500000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>27.462499999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42.087499999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42.087499999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>59.962499999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>66.462500000000006</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>97.174999999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>102.05</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>22.993749999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26.243749999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44.118749999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44.118749999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>21.06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21.06</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>24.31</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>24.31</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>38.935000000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>76.147499999999994</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.1937499999999899</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.43125</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.43125</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15.68125</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15.68125</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>69.712500000000006</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>96.232500000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.3624999999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>28.356249999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>34.693750000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>34.693750000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>41.193750000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>56.55</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>56.55</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>56.55</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>29.412500000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>29.412500000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>32.662500000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>49.887500000000003</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>56.387500000000003</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>56.387500000000003</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>14.625</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>16.087499999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>26.893749999999901</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>41.518749999999997</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43.712499999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>58.337499999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>64.837500000000006</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>71.337500000000006</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>82.257499999999993</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>82.257499999999993</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>110.69499999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>117.0325</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>8.125</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>8.125</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.375</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>28.193750000000001</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>34.693750000000001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>65.40625</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>70.866249999999994</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>26.26</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>26.26</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>52.422499999999999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>55.672499999999999</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>55.672499999999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>58.922499999999999</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>91.422499999999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>91.422499999999999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>97.922499999999999</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>128.63499999999999</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>134.095</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>134.095</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>155.155</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>155.155</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>155.155</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>34.384999999999998</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>36.578749999999999</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>39.828749999999999</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>39.828749999999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>72.328749999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>78.828749999999999</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>94.185000000000002</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>99.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>99.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>5.3624999999999998</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>11.862500000000001</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>11.862500000000001</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>15.112500000000001</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>31.931249999999999</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>38.431249999999999</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>47.141249999999999</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>76.472499999999997</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>22.993749999999999</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>37.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>45.743749999999999</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>68.737499999999997</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>71.987499999999997</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>75.237499999999997</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>105.94999999999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C15E-4A2C-8307-4062D2034C2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stir_daily_system_wide!$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MT_STIR_Sum_Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>stir_daily_system_wide!$Y$2:$Y$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="173"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>76.212500000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>76.212500000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>35.75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53.625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>60.125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>90.837500000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>90.837500000000006</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>22.993749999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26.243749999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>29.493749999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44.118749999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44.118749999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>50.618749999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>21.06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21.06</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>24.31</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>24.31</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>38.935000000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>76.147499999999994</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.6537499999999996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>17.891249999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>17.891249999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21.141249999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>21.141249999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>37.96</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44.46</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>75.172499999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>107.1525</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>26.243749999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>32.581249999999997</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>32.581249999999997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>39.081249999999997</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>54.4375</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>54.4375</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>54.4375</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>29.412500000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>31.606249999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>34.856250000000003</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>52.081249999999997</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>58.581249999999997</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>58.581249999999997</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>14.625</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>16.087499999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>26.893749999999901</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>41.518749999999997</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43.712499999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>58.337499999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>64.837500000000006</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>71.337500000000006</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>82.257499999999993</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>82.257499999999993</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>110.69499999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>117.0325</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>21.856249999999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>17.875</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>17.875</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>21.125</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>35.75</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>37.943750000000001</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>44.443750000000001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>75.15625</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>80.616249999999994</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>40.884999999999998</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>40.884999999999998</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>44.134999999999998</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>47.384999999999998</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>47.384999999999998</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>50.634999999999998</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>83.134999999999906</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>83.134999999999906</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>89.634999999999906</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>120.3475</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>125.807499999999</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>125.807499999999</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>146.86750000000001</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>146.86750000000001</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>146.86750000000001</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>29.51</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>31.703749999999999</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>34.953749999999999</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>34.953749999999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>67.453749999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>73.953749999999999</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>89.31</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>94.77</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>94.77</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>24.05</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>26.243749999999999</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>32.743749999999999</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>32.743749999999999</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>35.993749999999999</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>52.8125</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>59.3125</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>68.022499999999994</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>97.353750000000005</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2.1937499999999899</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>20.068750000000001</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>20.068750000000001</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>43.0625</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>46.3125</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>49.5625</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>80.275000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C15E-4A2C-8307-4062D2034C2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1769903087"/>
+        <c:axId val="1769904047"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1769903087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769904047"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1769904047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769903087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11593,6 +13527,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -13198,6 +15172,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -13309,6 +15799,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA356C48-3E95-F456-7219-A00FC0EF235F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13636,11 +16162,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2A62A6-3D73-4CE5-ABB5-A10C35402FCA}">
   <dimension ref="A1:Z174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AR41" sqref="AR41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
added STIR effects graph and PPT
</commit_message>
<xml_diff>
--- a/out/stir_daily_system_wide_with GRAPHS_22Oct25.xlsx
+++ b/out/stir_daily_system_wide_with GRAPHS_22Oct25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7d62234183fd3ba/Documents/GitHub/kerbel-long-term-impacts/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{3109FC4A-BD15-44FB-B1BB-C01FAB71276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EDFD4D9-34B1-44C7-A3E4-6655D2C4A1AD}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{3109FC4A-BD15-44FB-B1BB-C01FAB71276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B51F7A19-4EAD-5856-B5B2-4BA41BA417C6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{95A4D3B7-9F89-4514-B226-E93CDF5B25B1}"/>
+    <workbookView xWindow="-28695" yWindow="2340" windowWidth="28800" windowHeight="13155" xr2:uid="{95A4D3B7-9F89-4514-B226-E93CDF5B25B1}"/>
   </bookViews>
   <sheets>
     <sheet name="stir_daily_system_wide" sheetId="1" r:id="rId1"/>

</xml_diff>